<commit_message>
Update BOM-speeduino compatible PCB for m52 rev3.1 (PCBWay).xlsx
</commit_message>
<xml_diff>
--- a/m52_PnP/Rev3.1 documents/BOM-speeduino compatible PCB for m52 rev3.1 (PCBWay).xlsx
+++ b/m52_PnP/Rev3.1 documents/BOM-speeduino compatible PCB for m52 rev3.1 (PCBWay).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m52_PnP\Rev3.1 documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D0FEB1-CBA8-4266-9595-F29F3F29913C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9CEEC1-BCF5-4907-BCD3-44718153988A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="4575" windowWidth="28800" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="345" windowWidth="27855" windowHeight="19650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -770,6 +770,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -779,7 +780,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1135,7 +1135,7 @@
   <dimension ref="A2:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1153,25 +1153,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="D2" s="22" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="D2" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
     </row>
     <row r="6" spans="1:9" ht="28.5" customHeight="1">
       <c r="A6" s="2" t="s">
@@ -1325,7 +1325,7 @@
       <c r="D11" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="22" t="s">
         <v>142</v>
       </c>
       <c r="F11" s="11" t="s">
@@ -1671,7 +1671,7 @@
         <v>145</v>
       </c>
       <c r="C24" s="8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>17</v>
@@ -1865,7 +1865,7 @@
       <c r="D31" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="22" t="s">
         <v>132</v>
       </c>
       <c r="F31" s="13" t="s">
@@ -2085,7 +2085,7 @@
       <c r="D39" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E39" s="25" t="s">
+      <c r="E39" s="22" t="s">
         <v>135</v>
       </c>
       <c r="F39" s="13" t="s">

</xml_diff>